<commit_message>
Added DMQL students list
</commit_message>
<xml_diff>
--- a/DIC_list_A.xlsx
+++ b/DIC_list_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanke\Quiz_Attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16EBF6F-74D4-411E-851D-B4B7701BA448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A9059B-52F7-4278-B784-55BA12CB7B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1170" windowWidth="27660" windowHeight="15030" xr2:uid="{DFA42607-8057-4023-8519-0A3EE59F9943}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>